<commit_message>
added header end user fixed generate pdf
</commit_message>
<xml_diff>
--- a/RIS (1).xlsx
+++ b/RIS (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DepEd CSJDM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\depedcsjdm_RIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386609F0-8EE9-43A6-B75E-54EA5FD0AD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC3C78D-1B48-4C08-AFC4-9E402BF0E672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3BDCB5C7-FB56-4D7F-8B93-33D723252A35}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="2" xr2:uid="{3BDCB5C7-FB56-4D7F-8B93-33D723252A35}"/>
   </bookViews>
   <sheets>
     <sheet name="RIS" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3311,6 +3322,146 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3320,34 +3471,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3367,131 +3503,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4525,40 +4536,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="147" t="s">
         <v>477</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="101"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="149"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="140" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="104"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="142"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="140" t="s">
         <v>479</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="142"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
@@ -4578,37 +4589,37 @@
       <c r="A5" s="27" t="s">
         <v>481</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="143" t="s">
         <v>479</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="106" t="s">
+      <c r="C5" s="143"/>
+      <c r="D5" s="144" t="s">
         <v>482</v>
       </c>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="107" t="str">
+      <c r="E5" s="144"/>
+      <c r="F5" s="144"/>
+      <c r="G5" s="145" t="str">
         <f>IF(C27="","",VLOOKUP(C27,'RESPON. CENTER CODE'!A:D,4,0))</f>
         <v>S1</v>
       </c>
-      <c r="H5" s="108"/>
+      <c r="H5" s="146"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B6" s="109" t="str">
+      <c r="B6" s="132" t="str">
         <f>IF(C27="","",VLOOKUP(C27,'RESPON. CENTER CODE'!A:D,3,0))</f>
         <v>SDS</v>
       </c>
-      <c r="C6" s="109"/>
+      <c r="C6" s="132"/>
       <c r="D6" s="28" t="s">
         <v>484</v>
       </c>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="111"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="133"/>
+      <c r="G6" s="133"/>
+      <c r="H6" s="134"/>
     </row>
     <row r="7" spans="1:17" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
@@ -4621,20 +4632,20 @@
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="155" t="s">
         <v>485</v>
       </c>
-      <c r="B8" s="113"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="115" t="s">
+      <c r="B8" s="156"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="158" t="s">
         <v>486</v>
       </c>
-      <c r="F8" s="116"/>
-      <c r="G8" s="112" t="s">
+      <c r="F8" s="159"/>
+      <c r="G8" s="155" t="s">
         <v>487</v>
       </c>
-      <c r="H8" s="117"/>
+      <c r="H8" s="160"/>
       <c r="K8" s="40"/>
       <c r="L8" s="40"/>
       <c r="M8" s="40"/>
@@ -4944,120 +4955,120 @@
       <c r="A22" s="27" t="s">
         <v>495</v>
       </c>
-      <c r="B22" s="118"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="119"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="151"/>
+      <c r="D22" s="151"/>
+      <c r="E22" s="151"/>
+      <c r="F22" s="151"/>
+      <c r="G22" s="151"/>
+      <c r="H22" s="152"/>
     </row>
     <row r="23" spans="1:17" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
-      <c r="B23" s="120"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="120"/>
-      <c r="E23" s="120"/>
-      <c r="F23" s="120"/>
-      <c r="G23" s="120"/>
-      <c r="H23" s="121"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="103"/>
     </row>
     <row r="24" spans="1:17" ht="3.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="78"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="122"/>
-      <c r="E24" s="122"/>
-      <c r="F24" s="122"/>
-      <c r="G24" s="122"/>
-      <c r="H24" s="123"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="105"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="124" t="s">
+      <c r="A25" s="106" t="s">
         <v>496</v>
       </c>
-      <c r="B25" s="125"/>
-      <c r="C25" s="128" t="s">
+      <c r="B25" s="153"/>
+      <c r="C25" s="110" t="s">
         <v>497</v>
       </c>
-      <c r="D25" s="130" t="s">
+      <c r="D25" s="112" t="s">
         <v>498</v>
       </c>
-      <c r="E25" s="131"/>
-      <c r="F25" s="130" t="s">
+      <c r="E25" s="113"/>
+      <c r="F25" s="112" t="s">
         <v>499</v>
       </c>
-      <c r="G25" s="131"/>
-      <c r="H25" s="134" t="s">
+      <c r="G25" s="113"/>
+      <c r="H25" s="116" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="126"/>
-      <c r="B26" s="127"/>
-      <c r="C26" s="129"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="133"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="133"/>
-      <c r="H26" s="135"/>
+      <c r="A26" s="108"/>
+      <c r="B26" s="154"/>
+      <c r="C26" s="111"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="114"/>
+      <c r="G26" s="115"/>
+      <c r="H26" s="117"/>
     </row>
     <row r="27" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="136" t="s">
+      <c r="A27" s="124" t="s">
         <v>501</v>
       </c>
-      <c r="B27" s="137"/>
+      <c r="B27" s="150"/>
       <c r="C27" s="67" t="s">
         <v>644</v>
       </c>
-      <c r="D27" s="138" t="s">
+      <c r="D27" s="126" t="s">
         <v>614</v>
       </c>
-      <c r="E27" s="139"/>
-      <c r="F27" s="140" t="s">
+      <c r="E27" s="127"/>
+      <c r="F27" s="128" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="140"/>
+      <c r="G27" s="128"/>
       <c r="H27" s="79" t="str">
         <f>IF(C27="","",C27)</f>
         <v>Ericson S. Sabacan PhD, EdD CESO V</v>
       </c>
     </row>
     <row r="28" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="136" t="s">
+      <c r="A28" s="124" t="s">
         <v>502</v>
       </c>
-      <c r="B28" s="137"/>
+      <c r="B28" s="150"/>
       <c r="C28" s="67" t="str">
         <f>IF(C27="","",VLOOKUP(C27,'RESPON. CENTER CODE'!A:D,2,0))</f>
         <v>Schools Division Superintendent</v>
       </c>
-      <c r="D28" s="141" t="s">
+      <c r="D28" s="129" t="s">
         <v>503</v>
       </c>
-      <c r="E28" s="141"/>
-      <c r="F28" s="142" t="str">
+      <c r="E28" s="129"/>
+      <c r="F28" s="130" t="str">
         <f>IF(F27="Jhon Artin C. Victoriano","AA VI","AAI")</f>
         <v>AA VI</v>
       </c>
-      <c r="G28" s="143"/>
+      <c r="G28" s="131"/>
       <c r="H28" s="69" t="str">
         <f>IF(C28="","",C28)</f>
         <v>Schools Division Superintendent</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="144" t="s">
+      <c r="A29" s="118" t="s">
         <v>504</v>
       </c>
-      <c r="B29" s="145"/>
+      <c r="B29" s="119"/>
       <c r="C29" s="68">
         <v>45063</v>
       </c>
-      <c r="D29" s="146"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="148"/>
-      <c r="G29" s="149"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="123"/>
       <c r="H29" s="70">
         <f>IF(C29="","",C29)</f>
         <v>45063</v>
@@ -5115,40 +5126,40 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="99" t="s">
+      <c r="A36" s="147" t="s">
         <v>477</v>
       </c>
-      <c r="B36" s="100"/>
-      <c r="C36" s="100"/>
-      <c r="D36" s="100"/>
-      <c r="E36" s="100"/>
-      <c r="F36" s="100"/>
-      <c r="G36" s="100"/>
-      <c r="H36" s="101"/>
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="148"/>
+      <c r="F36" s="148"/>
+      <c r="G36" s="148"/>
+      <c r="H36" s="149"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="102" t="s">
+      <c r="A37" s="140" t="s">
         <v>478</v>
       </c>
-      <c r="B37" s="103"/>
-      <c r="C37" s="103"/>
-      <c r="D37" s="103"/>
-      <c r="E37" s="103"/>
-      <c r="F37" s="103"/>
-      <c r="G37" s="103"/>
-      <c r="H37" s="104"/>
+      <c r="B37" s="141"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="141"/>
+      <c r="E37" s="141"/>
+      <c r="F37" s="141"/>
+      <c r="G37" s="141"/>
+      <c r="H37" s="142"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="102" t="s">
+      <c r="A38" s="140" t="s">
         <v>479</v>
       </c>
-      <c r="B38" s="103"/>
-      <c r="C38" s="103"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="103"/>
-      <c r="H38" s="104"/>
+      <c r="B38" s="141"/>
+      <c r="C38" s="141"/>
+      <c r="D38" s="141"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="141"/>
+      <c r="G38" s="141"/>
+      <c r="H38" s="142"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
@@ -5178,37 +5189,37 @@
       <c r="A41" s="27" t="s">
         <v>481</v>
       </c>
-      <c r="B41" s="105" t="s">
+      <c r="B41" s="143" t="s">
         <v>479</v>
       </c>
-      <c r="C41" s="105"/>
-      <c r="D41" s="106" t="s">
+      <c r="C41" s="143"/>
+      <c r="D41" s="144" t="s">
         <v>482</v>
       </c>
-      <c r="E41" s="106"/>
-      <c r="F41" s="106"/>
-      <c r="G41" s="107" t="str">
+      <c r="E41" s="144"/>
+      <c r="F41" s="144"/>
+      <c r="G41" s="145" t="str">
         <f>G5</f>
         <v>S1</v>
       </c>
-      <c r="H41" s="108"/>
+      <c r="H41" s="146"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="B42" s="109" t="str">
+      <c r="B42" s="132" t="str">
         <f>B6</f>
         <v>SDS</v>
       </c>
-      <c r="C42" s="109"/>
+      <c r="C42" s="132"/>
       <c r="D42" s="28" t="s">
         <v>484</v>
       </c>
-      <c r="E42" s="110"/>
-      <c r="F42" s="110"/>
-      <c r="G42" s="110"/>
-      <c r="H42" s="111"/>
+      <c r="E42" s="133"/>
+      <c r="F42" s="133"/>
+      <c r="G42" s="133"/>
+      <c r="H42" s="134"/>
     </row>
     <row r="43" spans="1:8" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
@@ -5221,20 +5232,20 @@
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="150" t="s">
+      <c r="A44" s="135" t="s">
         <v>485</v>
       </c>
-      <c r="B44" s="151"/>
-      <c r="C44" s="151"/>
-      <c r="D44" s="152"/>
-      <c r="E44" s="153" t="s">
+      <c r="B44" s="136"/>
+      <c r="C44" s="136"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="138" t="s">
         <v>486</v>
       </c>
-      <c r="F44" s="154"/>
-      <c r="G44" s="150" t="s">
+      <c r="F44" s="139"/>
+      <c r="G44" s="135" t="s">
         <v>487</v>
       </c>
-      <c r="H44" s="152"/>
+      <c r="H44" s="137"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="63" t="s">
@@ -5530,125 +5541,125 @@
       <c r="A58" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="B58" s="120"/>
-      <c r="C58" s="120"/>
-      <c r="D58" s="120"/>
-      <c r="E58" s="120"/>
-      <c r="F58" s="120"/>
-      <c r="G58" s="120"/>
-      <c r="H58" s="121"/>
+      <c r="B58" s="102"/>
+      <c r="C58" s="102"/>
+      <c r="D58" s="102"/>
+      <c r="E58" s="102"/>
+      <c r="F58" s="102"/>
+      <c r="G58" s="102"/>
+      <c r="H58" s="103"/>
     </row>
     <row r="59" spans="1:8" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
-      <c r="B59" s="120"/>
-      <c r="C59" s="120"/>
-      <c r="D59" s="120"/>
-      <c r="E59" s="120"/>
-      <c r="F59" s="120"/>
-      <c r="G59" s="120"/>
-      <c r="H59" s="121"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="102"/>
+      <c r="D59" s="102"/>
+      <c r="E59" s="102"/>
+      <c r="F59" s="102"/>
+      <c r="G59" s="102"/>
+      <c r="H59" s="103"/>
     </row>
     <row r="60" spans="1:8" ht="4.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
-      <c r="B60" s="122"/>
-      <c r="C60" s="122"/>
-      <c r="D60" s="122"/>
-      <c r="E60" s="122"/>
-      <c r="F60" s="122"/>
-      <c r="G60" s="122"/>
-      <c r="H60" s="123"/>
+      <c r="B60" s="104"/>
+      <c r="C60" s="104"/>
+      <c r="D60" s="104"/>
+      <c r="E60" s="104"/>
+      <c r="F60" s="104"/>
+      <c r="G60" s="104"/>
+      <c r="H60" s="105"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="124" t="s">
+      <c r="A61" s="106" t="s">
         <v>496</v>
       </c>
-      <c r="B61" s="156"/>
-      <c r="C61" s="128" t="s">
+      <c r="B61" s="107"/>
+      <c r="C61" s="110" t="s">
         <v>497</v>
       </c>
-      <c r="D61" s="130" t="s">
+      <c r="D61" s="112" t="s">
         <v>498</v>
       </c>
-      <c r="E61" s="131"/>
-      <c r="F61" s="130" t="s">
+      <c r="E61" s="113"/>
+      <c r="F61" s="112" t="s">
         <v>499</v>
       </c>
-      <c r="G61" s="131"/>
-      <c r="H61" s="134" t="s">
+      <c r="G61" s="113"/>
+      <c r="H61" s="116" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="126"/>
-      <c r="B62" s="157"/>
-      <c r="C62" s="129"/>
-      <c r="D62" s="132"/>
-      <c r="E62" s="133"/>
-      <c r="F62" s="132"/>
-      <c r="G62" s="133"/>
-      <c r="H62" s="135"/>
+      <c r="A62" s="108"/>
+      <c r="B62" s="109"/>
+      <c r="C62" s="111"/>
+      <c r="D62" s="114"/>
+      <c r="E62" s="115"/>
+      <c r="F62" s="114"/>
+      <c r="G62" s="115"/>
+      <c r="H62" s="117"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="136" t="s">
+      <c r="A63" s="124" t="s">
         <v>501</v>
       </c>
-      <c r="B63" s="155"/>
+      <c r="B63" s="125"/>
       <c r="C63" s="67" t="str">
         <f>IF(C27="","",C27)</f>
         <v>Ericson S. Sabacan PhD, EdD CESO V</v>
       </c>
-      <c r="D63" s="138" t="str">
+      <c r="D63" s="126" t="str">
         <f>D27</f>
         <v>MA. THERESA M. ROXAS</v>
       </c>
-      <c r="E63" s="139"/>
-      <c r="F63" s="140" t="str">
+      <c r="E63" s="127"/>
+      <c r="F63" s="128" t="str">
         <f>F27</f>
         <v>Jhon Artin C. Victoriano</v>
       </c>
-      <c r="G63" s="140"/>
+      <c r="G63" s="128"/>
       <c r="H63" s="79" t="str">
         <f>C63</f>
         <v>Ericson S. Sabacan PhD, EdD CESO V</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="136" t="s">
+      <c r="A64" s="124" t="s">
         <v>502</v>
       </c>
-      <c r="B64" s="155"/>
+      <c r="B64" s="125"/>
       <c r="C64" s="67" t="str">
         <f>IF(C28="","",C28)</f>
         <v>Schools Division Superintendent</v>
       </c>
-      <c r="D64" s="141" t="str">
+      <c r="D64" s="129" t="str">
         <f>D28</f>
         <v>AO IV (Supply)</v>
       </c>
-      <c r="E64" s="141"/>
-      <c r="F64" s="142" t="str">
+      <c r="E64" s="129"/>
+      <c r="F64" s="130" t="str">
         <f>F28</f>
         <v>AA VI</v>
       </c>
-      <c r="G64" s="143"/>
+      <c r="G64" s="131"/>
       <c r="H64" s="69" t="str">
         <f>C64</f>
         <v>Schools Division Superintendent</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="144" t="s">
+      <c r="A65" s="118" t="s">
         <v>504</v>
       </c>
-      <c r="B65" s="145"/>
+      <c r="B65" s="119"/>
       <c r="C65" s="68">
         <f>IF(C29="","",C29)</f>
         <v>45063</v>
       </c>
-      <c r="D65" s="146"/>
-      <c r="E65" s="147"/>
-      <c r="F65" s="148"/>
-      <c r="G65" s="149"/>
+      <c r="D65" s="120"/>
+      <c r="E65" s="121"/>
+      <c r="F65" s="122"/>
+      <c r="G65" s="123"/>
       <c r="H65" s="66">
         <f>C65</f>
         <v>45063</v>
@@ -5662,12 +5673,43 @@
     <protectedRange algorithmName="SHA-512" hashValue="0QC8jPvnC67Xp1GKxQrgI1rCMB4JK/BBfzds6Ik0cyVEE9m0uP3KP/GYcVmofUpWyCpNf/dpVhyFO0hI/MTkVg==" saltValue="F6OXR/5evwSwqmRxKryrlg==" spinCount="100000" sqref="F27:G29 F63:G64" name="Range3"/>
   </protectedRanges>
   <mergeCells count="52">
-    <mergeCell ref="B58:H60"/>
-    <mergeCell ref="A61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:E62"/>
-    <mergeCell ref="F61:G62"/>
-    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B22:H24"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="F25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="A65:B65"/>
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="F65:G65"/>
@@ -5677,43 +5719,12 @@
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="F64:G64"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B22:H24"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:E26"/>
-    <mergeCell ref="F25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B58:H60"/>
+    <mergeCell ref="A61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:E62"/>
+    <mergeCell ref="F61:G62"/>
+    <mergeCell ref="H61:H62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27:G27 F63:G63" xr:uid="{1D992E62-5EF9-4B76-B1F8-72B05F211CBE}">
@@ -7432,8 +7443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F705A1A2-AFB9-4F7C-9DA4-A2D5E7CD8039}">
   <dimension ref="A1:W926"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8361,7 +8372,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="160" t="s">
+      <c r="A65" s="101" t="s">
         <v>685</v>
       </c>
       <c r="B65" s="94" t="s">
@@ -8375,7 +8386,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="160" t="s">
+      <c r="A66" s="101" t="s">
         <v>687</v>
       </c>
       <c r="B66" s="94" t="s">
@@ -9314,16 +9325,16 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="158" t="s">
+      <c r="A133" s="99" t="s">
         <v>671</v>
       </c>
-      <c r="B133" s="158" t="s">
+      <c r="B133" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="C133" s="158" t="s">
+      <c r="C133" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="D133" s="159" t="s">
+      <c r="D133" s="100" t="s">
         <v>672</v>
       </c>
     </row>

</xml_diff>